<commit_message>
🔄 Actualización automática del index.html y Excel
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5861</t>
+          <t>5862</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,14 +508,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TERRADA 38</t>
+          <t>CHARCAS 3715</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>806976057</v>
+        <v>806976061</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>cables a baja altura</t>
+          <t>Cable en panza Cable cortado</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -537,20 +537,20 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 38, "cod_calle": 21021, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.468589", "y": "-34.629828"}, "direccion": "TERRADA 38, CABA", "nombre_calle": "TERRADA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3715, "cod_calle": 3219, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.417181", "y": "-34.588033"}, "direccion": "CHARCAS 3715, CABA", "nombre_calle": "CHARCAS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>-58.468589</v>
+        <v>-58.417181</v>
       </c>
       <c r="L2" t="n">
-        <v>-34.629828</v>
+        <v>-34.588033</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5862</t>
+          <t>5868</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -560,14 +560,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CHARCAS 3715</t>
+          <t>CONESA 4370</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>806976061</v>
+        <v>806976063</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cable en panza Cable cortado</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -589,37 +589,37 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3715, "cod_calle": 3219, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.417181", "y": "-34.588033"}, "direccion": "CHARCAS 3715, CABA", "nombre_calle": "CHARCAS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 4370, "cod_calle": 3155, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.477194", "y": "-34.545825"}, "direccion": "CONESA 4370, CABA", "nombre_calle": "CONESA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>-58.417181</v>
+        <v>-58.477194</v>
       </c>
       <c r="L3" t="n">
-        <v>-34.588033</v>
+        <v>-34.545825</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5868</t>
+          <t>341</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>1/12/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CONESA 4370</t>
+          <t>Giribone 1618</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>806976063</v>
+        <v>806976083</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>se encuentra un Cable en panza</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -641,37 +641,37 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4370, "cod_calle": 3155, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.477194", "y": "-34.545825"}, "direccion": "CONESA 4370, CABA", "nombre_calle": "CONESA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1618, "cod_calle": 7052, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.465007", "y": "-34.579572"}, "direccion": "GIRIBONE 1618, CABA", "nombre_calle": "GIRIBONE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>-58.477194</v>
+        <v>-58.465007</v>
       </c>
       <c r="L4" t="n">
-        <v>-34.545825</v>
+        <v>-34.579572</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1/12/2024</t>
+          <t>1/22/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Giribone 1618</t>
+          <t>Donato alvarez 2720</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>806976083</v>
+        <v>806997023</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>se encuentra un Cable en panza</t>
+          <t>tendido a baja altura</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -693,37 +693,37 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1618, "cod_calle": 7052, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.465007", "y": "-34.579572"}, "direccion": "GIRIBONE 1618, CABA", "nombre_calle": "GIRIBONE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2720, "cod_calle": 1055, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.469199", "y": "-34.592896"}, "direccion": "ALVAREZ, DONATO, TTE. GRAL. AV. 2720, CABA", "nombre_calle": "ALVAREZ, DONATO, TTE. GRAL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>-58.465007</v>
+        <v>-58.469199</v>
       </c>
       <c r="L5" t="n">
-        <v>-34.579572</v>
+        <v>-34.592896</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1/22/2024</t>
+          <t>2/2/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Donato alvarez 2720</t>
+          <t>Salguero 3421</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>806997023</v>
+        <v>806997030</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>tendido a baja altura</t>
+          <t>esquina de padre Múgica y Salguero</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -745,37 +745,37 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2720, "cod_calle": 1055, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.469199", "y": "-34.592896"}, "direccion": "ALVAREZ, DONATO, TTE. GRAL. AV. 2720, CABA", "nombre_calle": "ALVAREZ, DONATO, TTE. GRAL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3421, "cod_calle": 20012, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.401407", "y": "-34.572944"}, "direccion": "SALGUERO, JERONIMO 3421, CABA", "nombre_calle": "SALGUERO, JERONIMO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>-58.469199</v>
+        <v>-58.401407</v>
       </c>
       <c r="L6" t="n">
-        <v>-34.592896</v>
+        <v>-34.572944</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1288</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2/2/2024</t>
+          <t>4/3/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Salguero 3421</t>
+          <t>Juan Vucetich 500</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>806997030</v>
+        <v>806998788</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>esquina de padre Múgica y Salguero</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -797,37 +797,37 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3421, "cod_calle": 20012, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.401407", "y": "-34.572944"}, "direccion": "SALGUERO, JERONIMO 3421, CABA", "nombre_calle": "SALGUERO, JERONIMO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 500, "cod_calle": 23078, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.484997", "y": "-34.641055"}, "direccion": "VUCETICH, JUAN 500, CABA", "nombre_calle": "VUCETICH, JUAN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>-58.401407</v>
+        <v>-58.484997</v>
       </c>
       <c r="L7" t="n">
-        <v>-34.572944</v>
+        <v>-34.641055</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1288</t>
+          <t>907</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/3/2024</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Juan Vucetich 500</t>
+          <t>Estados Unidos 1154</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>806998788</v>
+        <v>806999360</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -849,37 +849,37 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 500, "cod_calle": 23078, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.484997", "y": "-34.641055"}, "direccion": "VUCETICH, JUAN 500, CABA", "nombre_calle": "VUCETICH, JUAN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1154, "cod_calle": 5087, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.382309", "y": "-34.618589"}, "direccion": "ESTADOS UNIDOS 1154, CABA", "nombre_calle": "ESTADOS UNIDOS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>-58.484997</v>
+        <v>-58.382309</v>
       </c>
       <c r="L8" t="n">
-        <v>-34.641055</v>
+        <v>-34.618589</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>907</t>
+          <t>1620</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>5/3/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Estados Unidos 1154</t>
+          <t>Brandsen 2053</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>806999360</v>
+        <v>806999451</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -901,37 +901,37 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1154, "cod_calle": 5087, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.382309", "y": "-34.618589"}, "direccion": "ESTADOS UNIDOS 1154, CABA", "nombre_calle": "ESTADOS UNIDOS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2053, "cod_calle": 2110, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.379679", "y": "-34.638321"}, "direccion": "BRANDSEN 2053, CABA", "nombre_calle": "BRANDSEN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>-58.382309</v>
+        <v>-58.379679</v>
       </c>
       <c r="L9" t="n">
-        <v>-34.618589</v>
+        <v>-34.638321</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1620</t>
+          <t>1483</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5/3/2024</t>
+          <t>5/6/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Brandsen 2053</t>
+          <t>Figueroa Alcorta 5851</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E10" t="n">
-        <v>806999451</v>
+        <v>806999695</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>cables expuestos. Tendido cortado en el piso</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -953,20 +953,20 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2053, "cod_calle": 2110, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.379679", "y": "-34.638321"}, "direccion": "BRANDSEN 2053, CABA", "nombre_calle": "BRANDSEN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 5851, "cod_calle": 6025, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.428737", "y": "-34.558193"}, "direccion": "FIGUEROA ALCORTA, PRES. AV. 5851, CABA", "nombre_calle": "FIGUEROA ALCORTA, PRES. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>-58.379679</v>
+        <v>-58.428737</v>
       </c>
       <c r="L10" t="n">
-        <v>-34.638321</v>
+        <v>-34.558193</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1483</t>
+          <t>1618</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -976,14 +976,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Figueroa Alcorta 5851</t>
+          <t>Pola 2769</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E11" t="n">
-        <v>806999695</v>
+        <v>806999869</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>cables expuestos. Tendido cortado en el piso</t>
+          <t>Cables cortados - posible riesgo electrico</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1005,37 +1005,37 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5851, "cod_calle": 6025, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.428737", "y": "-34.558193"}, "direccion": "FIGUEROA ALCORTA, PRES. AV. 5851, CABA", "nombre_calle": "FIGUEROA ALCORTA, PRES. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2769, "cod_calle": 17105, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.482974", "y": "-34.663531"}, "direccion": "POLA 2769, CABA", "nombre_calle": "POLA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>-58.428737</v>
+        <v>-58.482974</v>
       </c>
       <c r="L11" t="n">
-        <v>-34.558193</v>
+        <v>-34.663531</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1618</t>
+          <t>1903</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5/6/2024</t>
+          <t>5/22/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Pola 2769</t>
+          <t>Av. Valentín Alsina 1220</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E12" t="n">
-        <v>806999869</v>
+        <v>807000180</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Cables cortados - posible riesgo electrico</t>
+          <t>Activos/nodos colgado del tendido</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1057,37 +1057,37 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2769, "cod_calle": 17105, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.482974", "y": "-34.663531"}, "direccion": "POLA 2769, CABA", "nombre_calle": "POLA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1220, "cod_calle": 1047, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441366", "y": "-34.558686"}, "direccion": "ALSINA, VALENTIN AV. 1220, CABA", "nombre_calle": "ALSINA, VALENTIN AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>-58.482974</v>
+        <v>-58.441366</v>
       </c>
       <c r="L12" t="n">
-        <v>-34.663531</v>
+        <v>-34.558686</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1903</t>
+          <t>2172</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/22/2024</t>
+          <t>6/19/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Av. Valentín Alsina 1220</t>
+          <t>JURAMENTO 1311</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>13</v>
       </c>
       <c r="E13" t="n">
-        <v>807000180</v>
+        <v>807000249</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Activos/nodos colgado del tendido</t>
+          <t>Tendido sobre medianera. Vecino solicita el retiro</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1109,37 +1109,37 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1220, "cod_calle": 1047, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441366", "y": "-34.558686"}, "direccion": "ALSINA, VALENTIN AV. 1220, CABA", "nombre_calle": "ALSINA, VALENTIN AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1311, "cod_calle": 10017, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.445759", "y": "-34.555489"}, "direccion": "JURAMENTO 1311, CABA", "nombre_calle": "JURAMENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>-58.441366</v>
+        <v>-58.445759</v>
       </c>
       <c r="L13" t="n">
-        <v>-34.558686</v>
+        <v>-34.555489</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2172</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6/19/2024</t>
+          <t>8/15/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>JURAMENTO 1311</t>
+          <t>Heredia 1423</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14" t="n">
-        <v>807000249</v>
+        <v>807000468</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tendido sobre medianera. Vecino solicita el retiro</t>
+          <t>se cortaron cables de servicio de su empresa en Heredia 1423</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1161,37 +1161,37 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1311, "cod_calle": 10017, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.445759", "y": "-34.555489"}, "direccion": "JURAMENTO 1311, CABA", "nombre_calle": "JURAMENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1423, "cod_calle": 8008, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464240", "y": "-34.576651"}, "direccion": "HEREDIA 1423, CABA", "nombre_calle": "HEREDIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>-58.445759</v>
+        <v>-58.46424</v>
       </c>
       <c r="L14" t="n">
-        <v>-34.555489</v>
+        <v>-34.576651</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2754</t>
+          <t>1493</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>9/11/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>EL SALVADOR 5935</t>
+          <t>Av. Piedra Buena 3491</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E15" t="n">
-        <v>807000434</v>
+        <v>807045221</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cable con panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1213,37 +1213,37 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5935, "cod_calle": 5050, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.438726", "y": "-34.580540"}, "direccion": "EL SALVADOR 5935, CABA", "nombre_calle": "EL SALVADOR", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3491, "cod_calle": 17077, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.491866", "y": "-34.674124"}, "direccion": "PIEDRA BUENA AV. 3491, CABA", "nombre_calle": "PIEDRA BUENA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>-58.438726</v>
+        <v>-58.491866</v>
       </c>
       <c r="L15" t="n">
-        <v>-34.58054</v>
+        <v>-34.674124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2738</t>
+          <t>2496</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>9/11/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 7031</t>
+          <t>DEL LIBERTADOR AV. 1544</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>807000449</v>
+        <v>807045233</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura obstaculiza contenedores</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1265,37 +1265,37 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 7031, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464641", "y": "-34.629284"}, "direccion": "RIVADAVIA AV. 7031, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1544, "cod_calle": 12107, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.395644", "y": "-34.583612"}, "direccion": "DEL LIBERTADOR AV. 1544, CABA", "nombre_calle": "DEL LIBERTADOR AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>-58.464641</v>
+        <v>-58.395644</v>
       </c>
       <c r="L16" t="n">
-        <v>-34.629284</v>
+        <v>-34.583612</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2870</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8/15/2024</t>
+          <t>9/16/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Heredia 1423</t>
+          <t>Iguazú 1598</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>807000468</v>
+        <v>807045248</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>se cortaron cables de servicio de su empresa en Heredia 1423</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1317,37 +1317,37 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1423, "cod_calle": 8008, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464240", "y": "-34.576651"}, "direccion": "HEREDIA 1423, CABA", "nombre_calle": "HEREDIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1598, "cod_calle": 9007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.402760", "y": "-34.655842"}, "direccion": "IGUAZU 1598, CABA", "nombre_calle": "IGUAZU", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>-58.46424</v>
+        <v>-58.40276</v>
       </c>
       <c r="L17" t="n">
-        <v>-34.576651</v>
+        <v>-34.655842</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1493</t>
+          <t>3564</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>9/11/2024</t>
+          <t>9/24/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Av. Piedra Buena 3491</t>
+          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 6335</t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>8</v>
       </c>
       <c r="E18" t="n">
-        <v>807045221</v>
+        <v>807045316</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>CABLES EN PANZA</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1369,37 +1369,37 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3491, "cod_calle": 17077, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.491866", "y": "-34.674124"}, "direccion": "PIEDRA BUENA AV. 3491, CABA", "nombre_calle": "PIEDRA BUENA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 6335, "cod_calle": 3195, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.474251", "y": "-34.686442"}, "direccion": "FERNANDEZ DE LA CRUZ, F., GRAL. AV. 6335, CABA", "nombre_calle": "FERNANDEZ DE LA CRUZ, F., GRAL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>-58.491866</v>
+        <v>-58.474251</v>
       </c>
       <c r="L18" t="n">
-        <v>-34.674124</v>
+        <v>-34.686442</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2496</t>
+          <t>2965</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>9/11/2024</t>
+          <t>10/3/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>DEL LIBERTADOR AV. 1544</t>
+          <t>ECHEVERRIA 3900</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>807045233</v>
+        <v>807045394</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Tendido a baja altura obstaculiza contenedores</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1421,37 +1421,37 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1544, "cod_calle": 12107, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.395644", "y": "-34.583612"}, "direccion": "DEL LIBERTADOR AV. 1544, CABA", "nombre_calle": "DEL LIBERTADOR AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3900, "cod_calle": 5007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.470342", "y": "-34.571598"}, "direccion": "ECHEVERRIA 3900, CABA", "nombre_calle": "ECHEVERRIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>-58.395644</v>
+        <v>-58.470342</v>
       </c>
       <c r="L19" t="n">
-        <v>-34.583612</v>
+        <v>-34.571598</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>5932</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>9/16/2024</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Iguazú 1598</t>
+          <t>HABANA 3246</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E20" t="n">
-        <v>807045248</v>
+        <v>807045429</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1473,37 +1473,37 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1598, "cod_calle": 9007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.402760", "y": "-34.655842"}, "direccion": "IGUAZU 1598, CABA", "nombre_calle": "IGUAZU", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3246, "cod_calle": 8001, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.504023", "y": "-34.592111"}, "direccion": "HABANA 3246, CABA", "nombre_calle": "HABANA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>-58.40276</v>
+        <v>-58.504023</v>
       </c>
       <c r="L20" t="n">
-        <v>-34.655842</v>
+        <v>-34.592111</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3069</t>
+          <t>5943</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>9/19/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PJE. CAPITAN SAMUEL SPIRO 5996</t>
+          <t>PAVON AV. 3745</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>807045256</v>
+        <v>807045515</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Tendido a abaja altura</t>
+          <t>Cable en panza cable cortado</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1525,37 +1525,37 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5996, "cod_calle": 20114, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.504798", "y": "-34.649012"}, "direccion": "SPIRO, SAMUEL, CAPITAN 5996, CABA", "nombre_calle": "SPIRO, SAMUEL, CAPITAN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3745, "cod_calle": 17038, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.417344", "y": "-34.630249"}, "direccion": "PAVON AV. 3745, CABA", "nombre_calle": "PAVON AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K21" t="n">
-        <v>-58.504798</v>
+        <v>-58.417344</v>
       </c>
       <c r="L21" t="n">
-        <v>-34.649012</v>
+        <v>-34.630249</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3564</t>
+          <t>5950</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>9/24/2024</t>
+          <t>5/30/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 6335</t>
+          <t>Moron 3350</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>807045316</v>
+        <v>807129443</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>CABLES EN PANZA</t>
+          <t>tendido en panza</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1577,37 +1577,37 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 6335, "cod_calle": 3195, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.474251", "y": "-34.686442"}, "direccion": "FERNANDEZ DE LA CRUZ, F., GRAL. AV. 6335, CABA", "nombre_calle": "FERNANDEZ DE LA CRUZ, F., GRAL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3350, "cod_calle": 13132, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.478062", "y": "-34.625668"}, "direccion": "MORON 3350, CABA", "nombre_calle": "MORON", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>-58.474251</v>
+        <v>-58.478062</v>
       </c>
       <c r="L22" t="n">
-        <v>-34.686442</v>
+        <v>-34.625668</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3640</t>
+          <t>5952</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>9/30/2024</t>
+          <t>5/30/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LOPE DE VEGA AV. 1621</t>
+          <t>YAPEYU 852</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>807045372</v>
+        <v>807129457</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza Cable cortado</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1629,37 +1629,37 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1621, "cod_calle": 12126, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.510761", "y": "-34.624864"}, "direccion": "LOPE DE VEGA AV. 1621, CABA", "nombre_calle": "LOPE DE VEGA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 852, "cod_calle": 26001, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.421330", "y": "-34.622193"}, "direccion": "YAPEYU 852, CABA", "nombre_calle": "YAPEYU", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>-58.510761</v>
+        <v>-58.42133</v>
       </c>
       <c r="L23" t="n">
-        <v>-34.624864</v>
+        <v>-34.622193</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2965</t>
+          <t>5958</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10/3/2024</t>
+          <t>5/30/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 3900</t>
+          <t>CUENCA 5240</t>
         </is>
       </c>
       <c r="D24" t="n">
         <v>12</v>
       </c>
       <c r="E24" t="n">
-        <v>807045394</v>
+        <v>807129476</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza Cable cortado</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1681,37 +1681,37 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3900, "cod_calle": 5007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.470342", "y": "-34.571598"}, "direccion": "ECHEVERRIA 3900, CABA", "nombre_calle": "ECHEVERRIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 5240, "cod_calle": 3200, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.510201", "y": "-34.584335"}, "direccion": "CUENCA 5240, CABA", "nombre_calle": "CUENCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>-58.470342</v>
+        <v>-58.510201</v>
       </c>
       <c r="L24" t="n">
-        <v>-34.571598</v>
+        <v>-34.584335</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5932</t>
+          <t>2929</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HABANA 3246</t>
+          <t>HUBAC 5719</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E25" t="n">
-        <v>807045429</v>
+        <v>807129541</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1733,37 +1733,37 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3246, "cod_calle": 8001, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.504023", "y": "-34.592111"}, "direccion": "HABANA 3246, CABA", "nombre_calle": "HABANA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 5719, "cod_calle": 8025, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.484043", "y": "-34.663129"}, "direccion": "HUBAC 5719, CABA", "nombre_calle": "HUBAC", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>-58.504023</v>
+        <v>-58.484043</v>
       </c>
       <c r="L25" t="n">
-        <v>-34.592111</v>
+        <v>-34.663129</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5943</t>
+          <t>3798</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PAVON AV. 3745</t>
+          <t>RIVADAVIA AV. 1559</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>807045515</v>
+        <v>807129585</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cable en panza cable cortado</t>
+          <t>Tendido a baja altura obstaculiza contenedores</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -1785,37 +1785,37 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3745, "cod_calle": 17038, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.417344", "y": "-34.630249"}, "direccion": "PAVON AV. 3745, CABA", "nombre_calle": "PAVON AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1559, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.388501", "y": "-34.608971"}, "direccion": "RIVADAVIA AV. 1559, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>-58.417344</v>
+        <v>-58.388501</v>
       </c>
       <c r="L26" t="n">
-        <v>-34.630249</v>
+        <v>-34.608971</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5950</t>
+          <t>3914</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/30/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Moron 3350</t>
+          <t>YRIGOYEN, HIPOLITO AV. 4251</t>
         </is>
       </c>
       <c r="D27" t="n">
         <v>5</v>
       </c>
       <c r="E27" t="n">
-        <v>807129443</v>
+        <v>807129638</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>tendido en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1837,37 +1837,37 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3350, "cod_calle": 13132, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.478062", "y": "-34.625668"}, "direccion": "MORON 3350, CABA", "nombre_calle": "MORON", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 4251, "cod_calle": 26005, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.426701", "y": "-34.614863"}, "direccion": "YRIGOYEN, HIPOLITO AV. 4251, CABA", "nombre_calle": "YRIGOYEN, HIPOLITO AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K27" t="n">
-        <v>-58.478062</v>
+        <v>-58.426701</v>
       </c>
       <c r="L27" t="n">
-        <v>-34.625668</v>
+        <v>-34.614863</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5952</t>
+          <t>1249</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/30/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>YAPEYU 852</t>
+          <t>ARGUIBEL 2887</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>807129457</v>
+        <v>807129649</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1881,7 +1881,8 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cable en panza Cable cortado</t>
+          <t xml:space="preserve">Cable en panza Cable caído desde el 2887 al 2909
+</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1889,37 +1890,37 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 852, "cod_calle": 26001, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.421330", "y": "-34.622193"}, "direccion": "YAPEYU 852, CABA", "nombre_calle": "YAPEYU", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2887, "cod_calle": 1154, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.429442", "y": "-34.571946"}, "direccion": "ARGUIBEL, ANDRES 2887, CABA", "nombre_calle": "ARGUIBEL, ANDRES", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>-58.42133</v>
+        <v>-58.429442</v>
       </c>
       <c r="L28" t="n">
-        <v>-34.622193</v>
+        <v>-34.571946</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5958</t>
+          <t>1913</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/30/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CUENCA 5240</t>
+          <t>Azopardo 1445</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E29" t="n">
-        <v>807129476</v>
+        <v>807129661</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1933,7 +1934,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Cable en panza Cable cortado</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -1941,20 +1942,20 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5240, "cod_calle": 3200, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.510201", "y": "-34.584335"}, "direccion": "CUENCA 5240, CABA", "nombre_calle": "CUENCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1445, "cod_calle": 1149, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.366654", "y": "-34.624373"}, "direccion": "AZOPARDO 1445, CABA", "nombre_calle": "AZOPARDO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>-58.510201</v>
+        <v>-58.366654</v>
       </c>
       <c r="L29" t="n">
-        <v>-34.584335</v>
+        <v>-34.624373</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3741</t>
+          <t>4117</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1964,14 +1965,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MURATURE 5259</t>
+          <t>ARISMENDI 2579</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E30" t="n">
-        <v>807129521</v>
+        <v>807129713</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1993,20 +1994,20 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5259, "cod_calle": 13143, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.504710", "y": "-34.631977"}, "direccion": "MURATURE 5259, CABA", "nombre_calle": "MURATURE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2579, "cod_calle": 1113, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.475553", "y": "-34.583791"}, "direccion": "ARISMENDI 2579, CABA", "nombre_calle": "ARISMENDI", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>-58.50471</v>
+        <v>-58.475553</v>
       </c>
       <c r="L30" t="n">
-        <v>-34.631977</v>
+        <v>-34.583791</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2892</t>
+          <t>4052</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2016,14 +2017,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>BAHIA BLANCA 1266</t>
+          <t>SANTA FE AV. 3443</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E31" t="n">
-        <v>807129530</v>
+        <v>807129714</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2037,7 +2038,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable a baja altura</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2045,20 +2046,20 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1266, "cod_calle": 2008, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.487874", "y": "-34.622216"}, "direccion": "BAHIA BLANCA 1266, CABA", "nombre_calle": "BAHIA BLANCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3443, "cod_calle": 20057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.413573", "y": "-34.586625"}, "direccion": "SANTA FE AV. 3443, CABA", "nombre_calle": "SANTA FE AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K31" t="n">
-        <v>-58.487874</v>
+        <v>-58.413573</v>
       </c>
       <c r="L31" t="n">
-        <v>-34.622216</v>
+        <v>-34.586625</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2929</t>
+          <t>4185</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2068,14 +2069,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>HUBAC 5719</t>
+          <t>AVELLANEDA 707</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E32" t="n">
-        <v>807129541</v>
+        <v>807129781</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2097,20 +2098,20 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5719, "cod_calle": 8025, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.484043", "y": "-34.663129"}, "direccion": "HUBAC 5719, CABA", "nombre_calle": "HUBAC", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 707, "cod_calle": 1141, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.440900", "y": "-34.614911"}, "direccion": "AVELLANEDA 707, CABA", "nombre_calle": "AVELLANEDA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K32" t="n">
-        <v>-58.484043</v>
+        <v>-58.4409</v>
       </c>
       <c r="L32" t="n">
-        <v>-34.663129</v>
+        <v>-34.614911</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3798</t>
+          <t>4323</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2120,14 +2121,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 1559</t>
+          <t>ROJAS 1285</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E33" t="n">
-        <v>807129585</v>
+        <v>807129801</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2141,7 +2142,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Tendido a baja altura obstaculiza contenedores</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2149,20 +2150,20 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1559, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.388501", "y": "-34.608971"}, "direccion": "RIVADAVIA AV. 1559, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1285, "cod_calle": 19075, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.448032", "y": "-34.606255"}, "direccion": "ROJAS 1285, CABA", "nombre_calle": "ROJAS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K33" t="n">
-        <v>-58.388501</v>
+        <v>-58.448032</v>
       </c>
       <c r="L33" t="n">
-        <v>-34.608971</v>
+        <v>-34.606255</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3914</t>
+          <t>4331</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2172,14 +2173,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>YRIGOYEN, HIPOLITO AV. 4251</t>
+          <t>REPUBLICA ARABE SIRIA 2699</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E34" t="n">
-        <v>807129638</v>
+        <v>807129809</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2193,7 +2194,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2201,20 +2202,20 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4251, "cod_calle": 26005, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.426701", "y": "-34.614863"}, "direccion": "YRIGOYEN, HIPOLITO AV. 4251, CABA", "nombre_calle": "YRIGOYEN, HIPOLITO AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2699, "cod_calle": 13016, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.415582", "y": "-34.583374"}, "direccion": "REPUBLICA ARABE SIRIA 2699, CABA", "nombre_calle": "REPUBLICA ARABE SIRIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K34" t="n">
-        <v>-58.426701</v>
+        <v>-58.415582</v>
       </c>
       <c r="L34" t="n">
-        <v>-34.614863</v>
+        <v>-34.583374</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1249</t>
+          <t>4276</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2224,14 +2225,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ARGUIBEL 2887</t>
+          <t>RABANAL, FRANCISCO, INTENDENTE AV. 3218</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
-        <v>807129649</v>
+        <v>807129816</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2245,8 +2246,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cable en panza Cable caído desde el 2887 al 2909
-</t>
+          <t>Tendido a baja altura conectado a camaras de seguridad</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -2254,20 +2254,20 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2887, "cod_calle": 1154, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.429442", "y": "-34.571946"}, "direccion": "ARGUIBEL, ANDRES 2887, CABA", "nombre_calle": "ARGUIBEL, ANDRES", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3218, "cod_calle": 19057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.438980", "y": "-34.665628"}, "direccion": "RABANAL, FRANCISCO, INTENDENTE AV. 3218, CABA", "nombre_calle": "RABANAL, FRANCISCO, INTENDENTE AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>-58.429442</v>
+        <v>-58.43898</v>
       </c>
       <c r="L35" t="n">
-        <v>-34.571946</v>
+        <v>-34.665628</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1913</t>
+          <t>4232</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2277,14 +2277,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Azopardo 1445</t>
+          <t>ROSARIO 242</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E36" t="n">
-        <v>807129661</v>
+        <v>807129862</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -2306,20 +2306,20 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1445, "cod_calle": 1149, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.366654", "y": "-34.624373"}, "direccion": "AZOPARDO 1445, CABA", "nombre_calle": "AZOPARDO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 242, "cod_calle": 19086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.432407", "y": "-34.618860"}, "direccion": "ROSARIO 242, CABA", "nombre_calle": "ROSARIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K36" t="n">
-        <v>-58.366654</v>
+        <v>-58.432407</v>
       </c>
       <c r="L36" t="n">
-        <v>-34.624373</v>
+        <v>-34.61886</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4117</t>
+          <t>4424</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2329,14 +2329,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ARISMENDI 2579</t>
+          <t>MARTI, JOSE 1080</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E37" t="n">
-        <v>807129713</v>
+        <v>807129895</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2358,20 +2358,20 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2579, "cod_calle": 1113, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.475553", "y": "-34.583791"}, "direccion": "ARISMENDI 2579, CABA", "nombre_calle": "ARISMENDI", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1080, "cod_calle": 13034, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464919", "y": "-34.643455"}, "direccion": "MARTI, JOSE 1080, CABA", "nombre_calle": "MARTI, JOSE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K37" t="n">
-        <v>-58.475553</v>
+        <v>-58.464919</v>
       </c>
       <c r="L37" t="n">
-        <v>-34.583791</v>
+        <v>-34.643455</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4052</t>
+          <t>4233</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2381,14 +2381,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SANTA FE AV. 3443</t>
+          <t>ROSARIO 300</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>807129714</v>
+        <v>807129906</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2402,7 +2402,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Cable a baja altura</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2410,20 +2410,20 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3443, "cod_calle": 20057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.413573", "y": "-34.586625"}, "direccion": "SANTA FE AV. 3443, CABA", "nombre_calle": "SANTA FE AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 300, "cod_calle": 19086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.433225", "y": "-34.618958"}, "direccion": "ROSARIO 300, CABA", "nombre_calle": "ROSARIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>-58.413573</v>
+        <v>-58.433225</v>
       </c>
       <c r="L38" t="n">
-        <v>-34.586625</v>
+        <v>-34.618958</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4049</t>
+          <t>4520</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2433,14 +2433,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SOLER 4193</t>
+          <t>RIVADAVIA AV. 10240</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>807129730</v>
+        <v>807129916</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Cable a baja altura Cable cortado</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -2462,20 +2462,20 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4193, "cod_calle": 20104, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.420053", "y": "-34.590125"}, "direccion": "SOLER 4193, CABA", "nombre_calle": "SOLER", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 10240, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.507786", "y": "-34.638829"}, "direccion": "RIVADAVIA AV. 10240, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>-58.420053</v>
+        <v>-58.507786</v>
       </c>
       <c r="L39" t="n">
-        <v>-34.590125</v>
+        <v>-34.638829</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4185</t>
+          <t>4588</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2485,14 +2485,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AVELLANEDA 707</t>
+          <t>DE LOS INCAS AV. 3694</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>807129781</v>
+        <v>807129921</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -2514,20 +2514,20 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 707, "cod_calle": 1141, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.440900", "y": "-34.614911"}, "direccion": "AVELLANEDA 707, CABA", "nombre_calle": "AVELLANEDA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3694, "cod_calle": 4045, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464500", "y": "-34.575874"}, "direccion": "DE LOS INCAS AV. 3694, CABA", "nombre_calle": "DE LOS INCAS AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K40" t="n">
-        <v>-58.4409</v>
+        <v>-58.4645</v>
       </c>
       <c r="L40" t="n">
-        <v>-34.614911</v>
+        <v>-34.575874</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4323</t>
+          <t>4907</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2537,14 +2537,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ROJAS 1285</t>
+          <t>CASTRO BARROS 885</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>807129801</v>
+        <v>807129940</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -2566,20 +2566,20 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1285, "cod_calle": 19075, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.448032", "y": "-34.606255"}, "direccion": "ROJAS 1285, CABA", "nombre_calle": "ROJAS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 885, "cod_calle": 3096, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.419365", "y": "-34.622279"}, "direccion": "CASTRO BARROS 885, CABA", "nombre_calle": "CASTRO BARROS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K41" t="n">
-        <v>-58.448032</v>
+        <v>-58.419365</v>
       </c>
       <c r="L41" t="n">
-        <v>-34.606255</v>
+        <v>-34.622279</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4331</t>
+          <t>4973</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2589,14 +2589,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>REPUBLICA ARABE SIRIA 2699</t>
+          <t>CONCORDIA 132</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E42" t="n">
-        <v>807129809</v>
+        <v>807129942</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -2618,20 +2618,20 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2699, "cod_calle": 13016, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.415582", "y": "-34.583374"}, "direccion": "REPUBLICA ARABE SIRIA 2699, CABA", "nombre_calle": "REPUBLICA ARABE SIRIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 132, "cod_calle": 3151, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.476520", "y": "-34.630550"}, "direccion": "CONCORDIA 132, CABA", "nombre_calle": "CONCORDIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K42" t="n">
-        <v>-58.415582</v>
+        <v>-58.47652</v>
       </c>
       <c r="L42" t="n">
-        <v>-34.583374</v>
+        <v>-34.63055</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4276</t>
+          <t>2225</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2641,14 +2641,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RABANAL, FRANCISCO, INTENDENTE AV. 3218</t>
+          <t>QUINQUELA MARTIN, BENITO 1282</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>807129816</v>
+        <v>807129962</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Tendido a baja altura conectado a camaras de seguridad</t>
+          <t>Tendido aereo a baja altura</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -2670,20 +2670,20 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3218, "cod_calle": 19057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.438980", "y": "-34.665628"}, "direccion": "RABANAL, FRANCISCO, INTENDENTE AV. 3218, CABA", "nombre_calle": "RABANAL, FRANCISCO, INTENDENTE AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1282, "cod_calle": 1137, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.368383", "y": "-34.642920"}, "direccion": "QUINQUELA MARTIN, BENITO 1282, CABA", "nombre_calle": "QUINQUELA MARTIN, BENITO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K43" t="n">
-        <v>-58.43898</v>
+        <v>-58.368383</v>
       </c>
       <c r="L43" t="n">
-        <v>-34.665628</v>
+        <v>-34.64292</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4386</t>
+          <t>5005</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2693,14 +2693,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>PUMACAHUA 197</t>
+          <t>CORDOBA AV. 2683</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E44" t="n">
-        <v>807129827</v>
+        <v>807129998</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Tendido abaja altura</t>
+          <t>CABLE A BAJA ALTURA</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2722,20 +2722,20 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 197, "cod_calle": 17136, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.454113", "y": "-34.628499"}, "direccion": "PUMACAHUA 197, CABA", "nombre_calle": "PUMACAHUA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2683, "cod_calle": 3165, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.405111", "y": "-34.597951"}, "direccion": "CORDOBA AV. 2683, CABA", "nombre_calle": "CORDOBA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K44" t="n">
-        <v>-58.454113</v>
+        <v>-58.405111</v>
       </c>
       <c r="L44" t="n">
-        <v>-34.628499</v>
+        <v>-34.597951</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4400</t>
+          <t>4870</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2745,14 +2745,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Av Dorrego 1430</t>
+          <t>ARAOZ DE LAMADRID, GREGORIO, GRAL. 283</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>807129846</v>
+        <v>807130010</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>tendido aéreo y nodo  a baja altura</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -2774,20 +2774,20 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1430, "cod_calle": 4089, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.445071", "y": "-34.585201"}, "direccion": "DORREGO AV. 1430, CABA", "nombre_calle": "DORREGO AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 283, "cod_calle": 1163, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.356207", "y": "-34.636226"}, "direccion": "ARAOZ DE LAMADRID, GREGORIO, GRAL. 283, CABA", "nombre_calle": "ARAOZ DE LAMADRID, GREGORIO, GRAL.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K45" t="n">
-        <v>-58.445071</v>
+        <v>-58.356207</v>
       </c>
       <c r="L45" t="n">
-        <v>-34.585201</v>
+        <v>-34.636226</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>4232</t>
+          <t>4825</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2797,14 +2797,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ROSARIO 242</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 461</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>807129862</v>
+        <v>807130034</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2826,20 +2826,20 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 242, "cod_calle": 19086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.432407", "y": "-34.618860"}, "direccion": "ROSARIO 242, CABA", "nombre_calle": "ROSARIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 461, "cod_calle": 2099, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.457458", "y": "-34.633218"}, "direccion": "BONORINO, ESTEBAN, CNEL. AV. 461, CABA", "nombre_calle": "BONORINO, ESTEBAN, CNEL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K46" t="n">
-        <v>-58.432407</v>
+        <v>-58.457458</v>
       </c>
       <c r="L46" t="n">
-        <v>-34.61886</v>
+        <v>-34.633218</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4424</t>
+          <t>4778</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2849,14 +2849,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MARTI, JOSE 1080</t>
+          <t>ITUZAINGO 870</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E47" t="n">
-        <v>807129895</v>
+        <v>807130040</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2878,20 +2878,20 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1080, "cod_calle": 13034, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464919", "y": "-34.643455"}, "direccion": "MARTI, JOSE 1080, CABA", "nombre_calle": "MARTI, JOSE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 870, "cod_calle": 9029, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.375676", "y": "-34.631856"}, "direccion": "ITUZAINGO 870, CABA", "nombre_calle": "ITUZAINGO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K47" t="n">
-        <v>-58.464919</v>
+        <v>-58.375676</v>
       </c>
       <c r="L47" t="n">
-        <v>-34.643455</v>
+        <v>-34.631856</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>4488</t>
+          <t>4733</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2901,14 +2901,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>EL SALVADOR 5821</t>
+          <t>MEXICO 544</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>807129901</v>
+        <v>807130091</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2930,20 +2930,20 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5821, "cod_calle": 5050, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.437601", "y": "-34.581474"}, "direccion": "EL SALVADOR 5821, CABA", "nombre_calle": "EL SALVADOR", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 544, "cod_calle": 13076, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.373929", "y": "-34.614923"}, "direccion": "MEXICO 544, CABA", "nombre_calle": "MEXICO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K48" t="n">
-        <v>-58.437601</v>
+        <v>-58.373929</v>
       </c>
       <c r="L48" t="n">
-        <v>-34.581474</v>
+        <v>-34.614923</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>4233</t>
+          <t>5939</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2953,14 +2953,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ROSARIO 300</t>
+          <t>FREIRE, RAMON, CAP. GRAL. 3650</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E49" t="n">
-        <v>807129906</v>
+        <v>807130098</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cables</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -2982,20 +2982,20 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 300, "cod_calle": 19086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.433225", "y": "-34.618958"}, "direccion": "ROSARIO 300, CABA", "nombre_calle": "ROSARIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3650, "cod_calle": 6057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.476430", "y": "-34.552826"}, "direccion": "FREIRE, RAMON, CAP. GRAL. 3650, CABA", "nombre_calle": "FREIRE, RAMON, CAP. GRAL.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K49" t="n">
-        <v>-58.433225</v>
+        <v>-58.47643</v>
       </c>
       <c r="L49" t="n">
-        <v>-34.618958</v>
+        <v>-34.552826</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>4520</t>
+          <t>4711</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3005,14 +3005,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 10240</t>
+          <t>CONDE 1378</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E50" t="n">
-        <v>807129916</v>
+        <v>807130108</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Tendido a baja altura obstaculiza cruza la calle obstaculiza alzamiento de contenedores</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -3034,20 +3034,20 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 10240, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.507786", "y": "-34.638829"}, "direccion": "RIVADAVIA AV. 10240, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1378, "cod_calle": 3153, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.457422", "y": "-34.574290"}, "direccion": "CONDE 1378, CABA", "nombre_calle": "CONDE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K50" t="n">
-        <v>-58.507786</v>
+        <v>-58.457422</v>
       </c>
       <c r="L50" t="n">
-        <v>-34.638829</v>
+        <v>-34.57429</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>4588</t>
+          <t>4695</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -3057,14 +3057,14 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DE LOS INCAS AV. 3694</t>
+          <t>CATAMARCA 359</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E51" t="n">
-        <v>807129921</v>
+        <v>807130114</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura y maraña de cables frente a Escuela</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -3086,20 +3086,20 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3694, "cod_calle": 4045, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.464500", "y": "-34.575874"}, "direccion": "DE LOS INCAS AV. 3694, CABA", "nombre_calle": "DE LOS INCAS AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 359, "cod_calle": 3100, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.406342", "y": "-34.614316"}, "direccion": "CATAMARCA 359, CABA", "nombre_calle": "CATAMARCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K51" t="n">
-        <v>-58.4645</v>
+        <v>-58.406342</v>
       </c>
       <c r="L51" t="n">
-        <v>-34.575874</v>
+        <v>-34.614316</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>4907</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3109,14 +3109,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CASTRO BARROS 885</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E52" t="n">
-        <v>807129940</v>
+        <v>807130118</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza cable suelto caja colgando</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -3138,20 +3138,20 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 885, "cod_calle": 3096, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.419365", "y": "-34.622279"}, "direccion": "CASTRO BARROS 885, CABA", "nombre_calle": "CASTRO BARROS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3345, "cod_calle": 3200, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.496935", "y": "-34.599084"}, "direccion": "CUENCA 3345, CABA", "nombre_calle": "CUENCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K52" t="n">
-        <v>-58.419365</v>
+        <v>-58.496935</v>
       </c>
       <c r="L52" t="n">
-        <v>-34.622279</v>
+        <v>-34.599084</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>4973</t>
+          <t>4538</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3161,14 +3161,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CONCORDIA 132</t>
+          <t>CASTAÑARES AV. 2419</t>
         </is>
       </c>
       <c r="D53" t="n">
         <v>7</v>
       </c>
       <c r="E53" t="n">
-        <v>807129942</v>
+        <v>807130123</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3190,20 +3190,20 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 132, "cod_calle": 3151, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.476520", "y": "-34.630550"}, "direccion": "CONCORDIA 132, CABA", "nombre_calle": "CONCORDIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2419, "cod_calle": 3086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.447840", "y": "-34.645902"}, "direccion": "CASTAÑARES AV. 2419, CABA", "nombre_calle": "CASTAÑARES AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K53" t="n">
-        <v>-58.47652</v>
+        <v>-58.44784</v>
       </c>
       <c r="L53" t="n">
-        <v>-34.63055</v>
+        <v>-34.645902</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2225</t>
+          <t>4639</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -3213,14 +3213,14 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>QUINQUELA MARTIN, BENITO 1282</t>
+          <t>Avenida Valentin Alsina 1220</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E54" t="n">
-        <v>807129962</v>
+        <v>807130133</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Tendido aereo a baja altura</t>
+          <t>Cable cortado Cable en panza</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -3242,20 +3242,20 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1282, "cod_calle": 1137, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.368383", "y": "-34.642920"}, "direccion": "QUINQUELA MARTIN, BENITO 1282, CABA", "nombre_calle": "QUINQUELA MARTIN, BENITO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1220, "cod_calle": 1047, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441366", "y": "-34.558686"}, "direccion": "ALSINA, VALENTIN AV. 1220, CABA", "nombre_calle": "ALSINA, VALENTIN AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K54" t="n">
-        <v>-58.368383</v>
+        <v>-58.441366</v>
       </c>
       <c r="L54" t="n">
-        <v>-34.64292</v>
+        <v>-34.558686</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>4997</t>
+          <t>5052</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3265,14 +3265,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>EL SALVADOR 5826</t>
+          <t>NUEVA YORK 3083</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E55" t="n">
-        <v>807129967</v>
+        <v>807130144</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>cable en panza cable cortado</t>
+          <t>Cable a baja altura</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -3294,20 +3294,20 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5826, "cod_calle": 5050, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.437714", "y": "-34.581522"}, "direccion": "EL SALVADOR 5826, CABA", "nombre_calle": "EL SALVADOR", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3083, "cod_calle": 14027, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.499944", "y": "-34.592844"}, "direccion": "NUEVA YORK 3083, CABA", "nombre_calle": "NUEVA YORK", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K55" t="n">
-        <v>-58.437714</v>
+        <v>-58.499944</v>
       </c>
       <c r="L55" t="n">
-        <v>-34.581522</v>
+        <v>-34.592844</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5005</t>
+          <t>5068</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3317,14 +3317,14 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CORDOBA AV. 2683</t>
+          <t>Libertad 1651</t>
         </is>
       </c>
       <c r="D56" t="n">
         <v>2</v>
       </c>
       <c r="E56" t="n">
-        <v>807129998</v>
+        <v>807130168</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CABLE A BAJA ALTURA</t>
+          <t>CABLES A BAJA ALTURA</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -3346,20 +3346,20 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2683, "cod_calle": 3165, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.405111", "y": "-34.597951"}, "direccion": "CORDOBA AV. 2683, CABA", "nombre_calle": "CORDOBA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1651, "cod_calle": 12106, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.383143", "y": "-34.588905"}, "direccion": "LIBERTAD 1651, CABA", "nombre_calle": "LIBERTAD", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 1651, "cod_calle": 12107, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.396608", "y": "-34.583205"}, "direccion": "DEL LIBERTADOR AV. 1651, CABA", "nombre_calle": "DEL LIBERTADOR AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K56" t="n">
-        <v>-58.405111</v>
+        <v>-58.383143</v>
       </c>
       <c r="L56" t="n">
-        <v>-34.597951</v>
+        <v>-34.588905</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>4870</t>
+          <t>5463</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3369,14 +3369,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ARAOZ DE LAMADRID, GREGORIO, GRAL. 283</t>
+          <t>MENDOZA 2638</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E57" t="n">
-        <v>807130010</v>
+        <v>807130218</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -3398,20 +3398,20 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 283, "cod_calle": 1163, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.356207", "y": "-34.636226"}, "direccion": "ARAOZ DE LAMADRID, GREGORIO, GRAL. 283, CABA", "nombre_calle": "ARAOZ DE LAMADRID, GREGORIO, GRAL.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2638, "cod_calle": 13071, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.459768", "y": "-34.562467"}, "direccion": "MENDOZA 2638, CABA", "nombre_calle": "MENDOZA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 2638, "cod_calle": 13072, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.357901", "y": "-34.644795"}, "direccion": "DON PEDRO DE MENDOZA AV. 2638, CABA", "nombre_calle": "DON PEDRO DE MENDOZA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K57" t="n">
-        <v>-58.356207</v>
+        <v>-58.459768</v>
       </c>
       <c r="L57" t="n">
-        <v>-34.636226</v>
+        <v>-34.562467</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>4825</t>
+          <t>5552</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3421,14 +3421,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 461</t>
+          <t>AVELLANEDA 212</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58" t="n">
-        <v>807130034</v>
+        <v>807130265</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -3450,20 +3450,20 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 461, "cod_calle": 2099, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.457458", "y": "-34.633218"}, "direccion": "BONORINO, ESTEBAN, CNEL. AV. 461, CABA", "nombre_calle": "BONORINO, ESTEBAN, CNEL. AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 212, "cod_calle": 1141, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.433499", "y": "-34.612328"}, "direccion": "AVELLANEDA 212, CABA", "nombre_calle": "AVELLANEDA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K58" t="n">
-        <v>-58.457458</v>
+        <v>-58.433499</v>
       </c>
       <c r="L58" t="n">
-        <v>-34.633218</v>
+        <v>-34.612328</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>4778</t>
+          <t>5661</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3473,14 +3473,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ITUZAINGO 870</t>
+          <t>ENTRE RIOS AV. 1795</t>
         </is>
       </c>
       <c r="D59" t="n">
         <v>4</v>
       </c>
       <c r="E59" t="n">
-        <v>807130040</v>
+        <v>807130298</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>CABLES A BAJA ALTURA</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -3502,20 +3502,20 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 870, "cod_calle": 9029, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.375676", "y": "-34.631856"}, "direccion": "ITUZAINGO 870, CABA", "nombre_calle": "ITUZAINGO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1795, "cod_calle": 5061, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.391061", "y": "-34.629160"}, "direccion": "ENTRE RIOS AV. 1795, CABA", "nombre_calle": "ENTRE RIOS AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K59" t="n">
-        <v>-58.375676</v>
+        <v>-58.391061</v>
       </c>
       <c r="L59" t="n">
-        <v>-34.631856</v>
+        <v>-34.62916</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4733</t>
+          <t>5705</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -3525,14 +3525,14 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MEXICO 544</t>
+          <t>SARMIENTO 1411</t>
         </is>
       </c>
       <c r="D60" t="n">
         <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>807130091</v>
+        <v>807130344</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -3554,20 +3554,20 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 544, "cod_calle": 13076, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.373929", "y": "-34.614923"}, "direccion": "MEXICO 544, CABA", "nombre_calle": "MEXICO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1411, "cod_calle": 20074, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.386629", "y": "-34.605247"}, "direccion": "SARMIENTO 1411, CABA", "nombre_calle": "SARMIENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 1411, "cod_calle": 6049, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.456976", "y": "-34.608713"}, "direccion": "FRAGATA PRES. SARMIENTO 1411, CABA", "nombre_calle": "FRAGATA PRES. SARMIENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K60" t="n">
-        <v>-58.373929</v>
+        <v>-58.386629</v>
       </c>
       <c r="L60" t="n">
-        <v>-34.614923</v>
+        <v>-34.605247</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5939</t>
+          <t>5753</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3577,14 +3577,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>FREIRE, RAMON, CAP. GRAL. 3650</t>
+          <t>MARTINEZ, VICTOR 1579</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>807130098</v>
+        <v>807130360</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Cables</t>
+          <t>Tendido a muy baja altura</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -3606,20 +3606,20 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3650, "cod_calle": 6057, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.476430", "y": "-34.552826"}, "direccion": "FREIRE, RAMON, CAP. GRAL. 3650, CABA", "nombre_calle": "FREIRE, RAMON, CAP. GRAL.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1579, "cod_calle": 13044, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.439404", "y": "-34.638290"}, "direccion": "MARTINEZ, VICTOR 1579, CABA", "nombre_calle": "MARTINEZ, VICTOR", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K61" t="n">
-        <v>-58.47643</v>
+        <v>-58.439404</v>
       </c>
       <c r="L61" t="n">
-        <v>-34.552826</v>
+        <v>-34.63829</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>4711</t>
+          <t>5761</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -3629,14 +3629,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CONDE 1378</t>
+          <t>MONTES DE OCA, MANUEL AV. 51</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E62" t="n">
-        <v>807130108</v>
+        <v>807130363</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tendido a baja altura obstaculiza cruza la calle obstaculiza alzamiento de contenedores</t>
+          <t>Resto de cables al retirar poste columna</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -3658,20 +3658,20 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1378, "cod_calle": 3153, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.457422", "y": "-34.574290"}, "direccion": "CONDE 1378, CABA", "nombre_calle": "CONDE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 51, "cod_calle": 13115, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.377677", "y": "-34.629259"}, "direccion": "MONTES DE OCA, MANUEL AV. 51, CABA", "nombre_calle": "MONTES DE OCA, MANUEL AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K62" t="n">
-        <v>-58.457422</v>
+        <v>-58.377677</v>
       </c>
       <c r="L62" t="n">
-        <v>-34.57429</v>
+        <v>-34.629259</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>4695</t>
+          <t>5776</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3681,14 +3681,14 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CATAMARCA 359</t>
+          <t>RODRIGUEZ, MANUEL A., GENERAL 1363</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E63" t="n">
-        <v>807130114</v>
+        <v>807130375</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Tendido a baja altura y maraña de cables frente a Escuela</t>
+          <t>Cable cortado cable en panza</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -3710,20 +3710,20 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 359, "cod_calle": 3100, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.406342", "y": "-34.614316"}, "direccion": "CATAMARCA 359, CABA", "nombre_calle": "CATAMARCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1363, "cod_calle": 19068, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.449530", "y": "-34.606318"}, "direccion": "RODRIGUEZ, MANUEL A., GENERAL 1363, CABA", "nombre_calle": "RODRIGUEZ, MANUEL A., GENERAL", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K63" t="n">
-        <v>-58.406342</v>
+        <v>-58.44953</v>
       </c>
       <c r="L63" t="n">
-        <v>-34.614316</v>
+        <v>-34.606318</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5797</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3733,14 +3733,14 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>QUITO 4367</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E64" t="n">
-        <v>807130118</v>
+        <v>807130386</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cable en panza cable suelto caja colgando</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -3762,20 +3762,20 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3345, "cod_calle": 3200, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.496935", "y": "-34.599084"}, "direccion": "CUENCA 3345, CABA", "nombre_calle": "CUENCA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 4367, "cod_calle": 18018, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.428211", "y": "-34.617113"}, "direccion": "QUITO 4367, CABA", "nombre_calle": "QUITO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K64" t="n">
-        <v>-58.496935</v>
+        <v>-58.428211</v>
       </c>
       <c r="L64" t="n">
-        <v>-34.599084</v>
+        <v>-34.617113</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>4538</t>
+          <t>5685</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3785,14 +3785,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 2419</t>
+          <t>HUMBERTO 1° 2159</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E65" t="n">
-        <v>807130123</v>
+        <v>807130396</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>Cable cortado Cable en panza cable suelto</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -3814,20 +3814,20 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2419, "cod_calle": 3086, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.447840", "y": "-34.645902"}, "direccion": "CASTAÑARES AV. 2419, CABA", "nombre_calle": "CASTAÑARES AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 2159, "cod_calle": 8035, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.396414", "y": "-34.621740"}, "direccion": "HUMBERTO 1° 2159, CABA", "nombre_calle": "HUMBERTO 1°", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K65" t="n">
-        <v>-58.44784</v>
+        <v>-58.396414</v>
       </c>
       <c r="L65" t="n">
-        <v>-34.645902</v>
+        <v>-34.62174</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>4639</t>
+          <t>5778</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3837,14 +3837,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Avenida Valentin Alsina 1220</t>
+          <t>GUEMES 3772</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E66" t="n">
-        <v>807130133</v>
+        <v>807130403</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -3858,7 +3858,8 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Cable cortado Cable en panza</t>
+          <t xml:space="preserve">Cable en panza Cable cortado cables sueltos
+</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -3866,37 +3867,37 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1220, "cod_calle": 1047, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441366", "y": "-34.558686"}, "direccion": "ALSINA, VALENTIN AV. 1220, CABA", "nombre_calle": "ALSINA, VALENTIN AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3772, "cod_calle": 7098, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.415372", "y": "-34.587614"}, "direccion": "GUEMES 3772, CABA", "nombre_calle": "GUEMES", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K66" t="n">
-        <v>-58.441366</v>
+        <v>-58.415372</v>
       </c>
       <c r="L66" t="n">
-        <v>-34.558686</v>
+        <v>-34.587614</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>4238</t>
+          <t>5798</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GUATEMALA 5527</t>
+          <t>VALLESE, FELIPE 566</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E67" t="n">
-        <v>807130137</v>
+        <v>807150896</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -3910,7 +3911,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -3918,37 +3919,37 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5527, "cod_calle": 7093, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.431302", "y": "-34.580805"}, "direccion": "GUATEMALA 5527, CABA", "nombre_calle": "GUATEMALA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 566, "cod_calle": 23081, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441613", "y": "-34.611714"}, "direccion": "VALLESE, FELIPE 566, CABA", "nombre_calle": "VALLESE, FELIPE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K67" t="n">
-        <v>-58.431302</v>
+        <v>-58.441613</v>
       </c>
       <c r="L67" t="n">
-        <v>-34.580805</v>
+        <v>-34.611714</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>5052</t>
+          <t>5793</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>NUEVA YORK 3083</t>
+          <t>ACOSTA, MARIANO 1797</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E68" t="n">
-        <v>807130144</v>
+        <v>807150901</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -3962,7 +3963,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cable a baja altura</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -3970,37 +3971,37 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3083, "cod_calle": 14027, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.499944", "y": "-34.592844"}, "direccion": "NUEVA YORK 3083, CABA", "nombre_calle": "NUEVA YORK", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1797, "cod_calle": 1006, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.462895", "y": "-34.649436"}, "direccion": "ACOSTA, MARIANO 1797, CABA", "nombre_calle": "ACOSTA, MARIANO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K68" t="n">
-        <v>-58.499944</v>
+        <v>-58.462895</v>
       </c>
       <c r="L68" t="n">
-        <v>-34.592844</v>
+        <v>-34.649436</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>5060</t>
+          <t>3798</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SASTRE, MARCOS 5755</t>
+          <t>RIVADAVIA AV. 1559</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>807130148</v>
+        <v>807150911</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -4014,7 +4015,8 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t xml:space="preserve">Tendido a baja altura obstaculiza contenedores
+</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -4022,37 +4024,37 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5755, "cod_calle": 20079, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.520266", "y": "-34.624776"}, "direccion": "SASTRE, MARCOS 5755, CABA", "nombre_calle": "SASTRE, MARCOS", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1559, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.388501", "y": "-34.608971"}, "direccion": "RIVADAVIA AV. 1559, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K69" t="n">
-        <v>-58.520266</v>
+        <v>-58.388501</v>
       </c>
       <c r="L69" t="n">
-        <v>-34.624776</v>
+        <v>-34.608971</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>3220</t>
+          <t>2736</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>GONZALEZ, ELPIDIO 4587</t>
+          <t>LOZANO, PEDRO 3274</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70" t="n">
-        <v>807130164</v>
+        <v>807150915</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -4066,7 +4068,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Tendido aereo a baja altura</t>
+          <t>Cable en panza</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -4074,37 +4076,37 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4587, "cod_calle": 7065, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.500553", "y": "-34.621168"}, "direccion": "GONZALEZ, ELPIDIO 4587, CABA", "nombre_calle": "GONZALEZ, ELPIDIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 3274, "cod_calle": 12146, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.496208", "y": "-34.601968"}, "direccion": "LOZANO, PEDRO 3274, CABA", "nombre_calle": "LOZANO, PEDRO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K70" t="n">
-        <v>-58.500553</v>
+        <v>-58.496208</v>
       </c>
       <c r="L70" t="n">
-        <v>-34.621168</v>
+        <v>-34.601968</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>5068</t>
+          <t>5827</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Libertad 1651</t>
+          <t>HELGUERA 5800</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E71" t="n">
-        <v>807130168</v>
+        <v>807150917</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -4118,7 +4120,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>CABLES A BAJA ALTURA</t>
+          <t>Cable en panza Cable cortado</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -4126,37 +4128,37 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1651, "cod_calle": 12106, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.383143", "y": "-34.588905"}, "direccion": "LIBERTAD 1651, CABA", "nombre_calle": "LIBERTAD", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 1651, "cod_calle": 12107, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.396608", "y": "-34.583205"}, "direccion": "DEL LIBERTADOR AV. 1651, CABA", "nombre_calle": "DEL LIBERTADOR AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 5800, "cod_calle": 8007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.512650", "y": "-34.579347"}, "direccion": "HELGUERA 5800, CABA", "nombre_calle": "HELGUERA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K71" t="n">
-        <v>-58.383143</v>
+        <v>-58.51265</v>
       </c>
       <c r="L71" t="n">
-        <v>-34.588905</v>
+        <v>-34.579347</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>3222</t>
+          <t>1912</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>GONZALEZ, ELPIDIO 4742</t>
+          <t>PASEO COLON AV. 1633</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E72" t="n">
-        <v>807130180</v>
+        <v>807150925</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -4170,7 +4172,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Tendido aéreo a baja altura</t>
+          <t>Tendido a baja altura del lado del Parque Lezama</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -4178,37 +4180,37 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4742, "cod_calle": 7065, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.502568", "y": "-34.622344"}, "direccion": "GONZALEZ, ELPIDIO 4742, CABA", "nombre_calle": "GONZALEZ, ELPIDIO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1633, "cod_calle": 17028, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.367982", "y": "-34.626490"}, "direccion": "PASEO COLON AV. 1633, CABA", "nombre_calle": "PASEO COLON AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K72" t="n">
-        <v>-58.502568</v>
+        <v>-58.367982</v>
       </c>
       <c r="L72" t="n">
-        <v>-34.622344</v>
+        <v>-34.62649</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>5463</t>
+          <t>4582</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>MENDOZA 2638</t>
+          <t>SANTO TOME 5647</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>807130218</v>
+        <v>807150930</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -4222,7 +4224,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cable en panza</t>
+          <t>Tendido a baja altura</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -4230,37 +4232,37 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2638, "cod_calle": 13071, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.459768", "y": "-34.562467"}, "direccion": "MENDOZA 2638, CABA", "nombre_calle": "MENDOZA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 2638, "cod_calle": 13072, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.357901", "y": "-34.644795"}, "direccion": "DON PEDRO DE MENDOZA AV. 2638, CABA", "nombre_calle": "DON PEDRO DE MENDOZA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 5647, "cod_calle": 20068, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.518176", "y": "-34.624768"}, "direccion": "SANTO TOME 5647, CABA", "nombre_calle": "SANTO TOME", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K73" t="n">
-        <v>-58.459768</v>
+        <v>-58.518176</v>
       </c>
       <c r="L73" t="n">
-        <v>-34.562467</v>
+        <v>-34.624768</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>5497</t>
+          <t>807168088</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ZUVIRIA 16</t>
+          <t>Brandsen 1700</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>807130230</v>
+        <v>807168088</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -4274,45 +4276,45 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Tendido a baja altura</t>
+          <t>regularización y ordenamiento, retirando también todo aquel cableado y elementos que se encuentren en desuso</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 16, "cod_calle": 27026, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.426861", "y": "-34.628406"}, "direccion": "ZUVIRIA 16, CABA", "nombre_calle": "ZUVIRIA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 1700, "cod_calle": 2110, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.374618", "y": "-34.637891"}, "direccion": "BRANDSEN 1700, CABA", "nombre_calle": "BRANDSEN", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K74" t="n">
-        <v>-58.426861</v>
+        <v>-58.374618</v>
       </c>
       <c r="L74" t="n">
-        <v>-34.628406</v>
+        <v>-34.637891</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>5552</t>
+          <t>2111</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>AVELLANEDA 212</t>
+          <t>GUARANI 80</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>807130265</v>
+        <v>807187735</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -4334,37 +4336,37 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 212, "cod_calle": 1141, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.433499", "y": "-34.612328"}, "direccion": "AVELLANEDA 212, CABA", "nombre_calle": "AVELLANEDA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 80, "cod_calle": 7090, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.414238", "y": "-34.639684"}, "direccion": "GUARANI 80, CABA", "nombre_calle": "GUARANI", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K75" t="n">
-        <v>-58.433499</v>
+        <v>-58.414238</v>
       </c>
       <c r="L75" t="n">
-        <v>-34.612328</v>
+        <v>-34.639684</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>5635</t>
+          <t>4350</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ARENAL, CONCEPCION 3686</t>
+          <t>DE LOS CORRALES AV. 6574</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E76" t="n">
-        <v>807130288</v>
+        <v>807187728</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -4378,7 +4380,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cable en panza Cable cortado</t>
+          <t>Tendido a muy baja altura</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -4386,37 +4388,37 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3686, "cod_calle": 1103, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.447304", "y": "-34.585584"}, "direccion": "ARENAL, CONCEPCION 3686, CABA", "nombre_calle": "ARENAL, CONCEPCION", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 6574, "cod_calle": 4044, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.500618", "y": "-34.663119"}, "direccion": "DE LOS CORRALES AV. 6574, CABA", "nombre_calle": "DE LOS CORRALES AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K76" t="n">
-        <v>-58.447304</v>
+        <v>-58.500618</v>
       </c>
       <c r="L76" t="n">
-        <v>-34.585584</v>
+        <v>-34.663119</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>5661</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ENTRE RIOS AV. 1795</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E77" t="n">
-        <v>807130298</v>
+        <v>807187714</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -4430,7 +4432,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>CABLES A BAJA ALTURA</t>
+          <t>Cable en panza Cable cortado coincide con reclamo de columna mismo caso</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -4438,796 +4440,14 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1795, "cod_calle": 5061, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.391061", "y": "-34.629160"}, "direccion": "ENTRE RIOS AV. 1795, CABA", "nombre_calle": "ENTRE RIOS AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
+          <t>{"direccionesNormalizadas": [{"altura": 256, "cod_calle": 13032, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.425845", "y": "-34.616562"}, "direccion": "MARMOL, JOSE 256, CABA", "nombre_calle": "MARMOL, JOSE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
         </is>
       </c>
       <c r="K77" t="n">
-        <v>-58.391061</v>
+        <v>-58.425845</v>
       </c>
       <c r="L77" t="n">
-        <v>-34.62916</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>5705</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>SARMIENTO 1411</t>
-        </is>
-      </c>
-      <c r="D78" t="n">
-        <v>1</v>
-      </c>
-      <c r="E78" t="n">
-        <v>807130344</v>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Cable en panza</t>
-        </is>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1411, "cod_calle": 20074, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.386629", "y": "-34.605247"}, "direccion": "SARMIENTO 1411, CABA", "nombre_calle": "SARMIENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}, {"altura": 1411, "cod_calle": 6049, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.456976", "y": "-34.608713"}, "direccion": "FRAGATA PRES. SARMIENTO 1411, CABA", "nombre_calle": "FRAGATA PRES. SARMIENTO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K78" t="n">
-        <v>-58.386629</v>
-      </c>
-      <c r="L78" t="n">
-        <v>-34.605247</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>5753</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>MARTINEZ, VICTOR 1579</t>
-        </is>
-      </c>
-      <c r="D79" t="n">
-        <v>7</v>
-      </c>
-      <c r="E79" t="n">
-        <v>807130360</v>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Tendido a muy baja altura</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1579, "cod_calle": 13044, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.439404", "y": "-34.638290"}, "direccion": "MARTINEZ, VICTOR 1579, CABA", "nombre_calle": "MARTINEZ, VICTOR", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K79" t="n">
-        <v>-58.439404</v>
-      </c>
-      <c r="L79" t="n">
-        <v>-34.63829</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>5761</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>MONTES DE OCA, MANUEL AV. 51</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>4</v>
-      </c>
-      <c r="E80" t="n">
-        <v>807130363</v>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Resto de cables al retirar poste columna</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 51, "cod_calle": 13115, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.377677", "y": "-34.629259"}, "direccion": "MONTES DE OCA, MANUEL AV. 51, CABA", "nombre_calle": "MONTES DE OCA, MANUEL AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K80" t="n">
-        <v>-58.377677</v>
-      </c>
-      <c r="L80" t="n">
-        <v>-34.629259</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>5776</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>RODRIGUEZ, MANUEL A., GENERAL 1363</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>15</v>
-      </c>
-      <c r="E81" t="n">
-        <v>807130375</v>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Cable cortado cable en panza</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1363, "cod_calle": 19068, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.449530", "y": "-34.606318"}, "direccion": "RODRIGUEZ, MANUEL A., GENERAL 1363, CABA", "nombre_calle": "RODRIGUEZ, MANUEL A., GENERAL", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K81" t="n">
-        <v>-58.44953</v>
-      </c>
-      <c r="L81" t="n">
-        <v>-34.606318</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>5797</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>QUITO 4367</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>6</v>
-      </c>
-      <c r="E82" t="n">
-        <v>807130386</v>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Tendido a baja altura</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4367, "cod_calle": 18018, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.428211", "y": "-34.617113"}, "direccion": "QUITO 4367, CABA", "nombre_calle": "QUITO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K82" t="n">
-        <v>-58.428211</v>
-      </c>
-      <c r="L82" t="n">
-        <v>-34.617113</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>5685</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>HUMBERTO 1° 2159</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>3</v>
-      </c>
-      <c r="E83" t="n">
-        <v>807130396</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Cable cortado Cable en panza cable suelto</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 2159, "cod_calle": 8035, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.396414", "y": "-34.621740"}, "direccion": "HUMBERTO 1° 2159, CABA", "nombre_calle": "HUMBERTO 1°", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K83" t="n">
-        <v>-58.396414</v>
-      </c>
-      <c r="L83" t="n">
-        <v>-34.62174</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>5778</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>GUEMES 3772</t>
-        </is>
-      </c>
-      <c r="D84" t="n">
-        <v>14</v>
-      </c>
-      <c r="E84" t="n">
-        <v>807130403</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cable en panza Cable cortado cables sueltos
-</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3772, "cod_calle": 7098, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.415372", "y": "-34.587614"}, "direccion": "GUEMES 3772, CABA", "nombre_calle": "GUEMES", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K84" t="n">
-        <v>-58.415372</v>
-      </c>
-      <c r="L84" t="n">
-        <v>-34.587614</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>1919</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>6/2/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Lascano 4320</t>
-        </is>
-      </c>
-      <c r="D85" t="n">
-        <v>10</v>
-      </c>
-      <c r="E85" t="n">
-        <v>807130406</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Cables a baja altura</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 4320, "cod_calle": 12071, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.501222", "y": "-34.616015"}, "direccion": "LASCANO 4320, CABA", "nombre_calle": "LASCANO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K85" t="n">
-        <v>-58.501222</v>
-      </c>
-      <c r="L85" t="n">
-        <v>-34.616015</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>5798</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>VALLESE, FELIPE 566</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>6</v>
-      </c>
-      <c r="E86" t="n">
-        <v>807150896</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Tendido a baja altura</t>
-        </is>
-      </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 566, "cod_calle": 23081, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.441613", "y": "-34.611714"}, "direccion": "VALLESE, FELIPE 566, CABA", "nombre_calle": "VALLESE, FELIPE", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K86" t="n">
-        <v>-58.441613</v>
-      </c>
-      <c r="L86" t="n">
-        <v>-34.611714</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>5793</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>ACOSTA, MARIANO 1797</t>
-        </is>
-      </c>
-      <c r="D87" t="n">
-        <v>7</v>
-      </c>
-      <c r="E87" t="n">
-        <v>807150901</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Tendido a baja altura</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1797, "cod_calle": 1006, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.462895", "y": "-34.649436"}, "direccion": "ACOSTA, MARIANO 1797, CABA", "nombre_calle": "ACOSTA, MARIANO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K87" t="n">
-        <v>-58.462895</v>
-      </c>
-      <c r="L87" t="n">
-        <v>-34.649436</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>3798</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>RIVADAVIA AV. 1559</t>
-        </is>
-      </c>
-      <c r="D88" t="n">
-        <v>1</v>
-      </c>
-      <c r="E88" t="n">
-        <v>807150911</v>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Tendido a baja altura obstaculiza contenedores
-</t>
-        </is>
-      </c>
-      <c r="I88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1559, "cod_calle": 19046, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.388501", "y": "-34.608971"}, "direccion": "RIVADAVIA AV. 1559, CABA", "nombre_calle": "RIVADAVIA AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K88" t="n">
-        <v>-58.388501</v>
-      </c>
-      <c r="L88" t="n">
-        <v>-34.608971</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>2736</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>LOZANO, PEDRO 3274</t>
-        </is>
-      </c>
-      <c r="D89" t="n">
-        <v>11</v>
-      </c>
-      <c r="E89" t="n">
-        <v>807150915</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Cable en panza</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 3274, "cod_calle": 12146, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.496208", "y": "-34.601968"}, "direccion": "LOZANO, PEDRO 3274, CABA", "nombre_calle": "LOZANO, PEDRO", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K89" t="n">
-        <v>-58.496208</v>
-      </c>
-      <c r="L89" t="n">
-        <v>-34.601968</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>5827</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>HELGUERA 5800</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>12</v>
-      </c>
-      <c r="E90" t="n">
-        <v>807150917</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Cable en panza Cable cortado</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5800, "cod_calle": 8007, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.512650", "y": "-34.579347"}, "direccion": "HELGUERA 5800, CABA", "nombre_calle": "HELGUERA", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K90" t="n">
-        <v>-58.51265</v>
-      </c>
-      <c r="L90" t="n">
-        <v>-34.579347</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>1912</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>PASEO COLON AV. 1633</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>4</v>
-      </c>
-      <c r="E91" t="n">
-        <v>807150925</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Tendido a baja altura del lado del Parque Lezama</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 1633, "cod_calle": 17028, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.367982", "y": "-34.626490"}, "direccion": "PASEO COLON AV. 1633, CABA", "nombre_calle": "PASEO COLON AV.", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K91" t="n">
-        <v>-58.367982</v>
-      </c>
-      <c r="L91" t="n">
-        <v>-34.62649</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>4582</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>6/3/2025</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>SANTO TOME 5647</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>10</v>
-      </c>
-      <c r="E92" t="n">
-        <v>807150930</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Tendido a baja altura</t>
-        </is>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>{"direccionesNormalizadas": [{"altura": 5647, "cod_calle": 20068, "cod_calle_cruce": null, "cod_partido": "caba", "coordenadas": {"srid": 4326, "x": "-58.518176", "y": "-34.624768"}, "direccion": "SANTO TOME 5647, CABA", "nombre_calle": "SANTO TOME", "nombre_calle_cruce": "", "nombre_localidad": "CABA", "nombre_partido": "CABA", "tipo": "calle_altura"}]}</t>
-        </is>
-      </c>
-      <c r="K92" t="n">
-        <v>-58.518176</v>
-      </c>
-      <c r="L92" t="n">
-        <v>-34.624768</v>
+        <v>-34.616562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>